<commit_message>
HTML version of project implementation plan
</commit_message>
<xml_diff>
--- a/Jun 21 - WHS Assess 2 - Report/Project-Implementation-Plan.xlsx
+++ b/Jun 21 - WHS Assess 2 - Report/Project-Implementation-Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Webbies19\Jun 21 - WHS Assess 2 - Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D035F8-79CC-4CA6-93C8-1180C1059791}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272FDA22-500F-4A84-8B58-4DE6B89FA32A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B31CDE22-2818-4661-946A-C693AE7A7A2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B31CDE22-2818-4661-946A-C693AE7A7A2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -932,23 +932,62 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -956,46 +995,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1317,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C5695D-2648-4B59-B8F9-85A5774BF697}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C115" sqref="C108:C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,139 +1702,139 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="46">
         <v>1</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="47" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="48" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="32"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
+      <c r="A8" s="33">
         <v>2</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="36" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="41" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="44"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="42"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
-      <c r="B12" s="45"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="29"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="39">
         <v>3</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="31"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="36"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="39"/>
+      <c r="D17" s="32"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="40">
+      <c r="A18" s="33">
         <v>4</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="41" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="10" t="s">
@@ -1842,24 +1842,24 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42"/>
-      <c r="B20" s="45"/>
-      <c r="C20" s="29"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="A21" s="39">
         <v>5</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="27" t="s">
         <v>99</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1870,8 +1870,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="13" t="s">
         <v>42</v>
       </c>
@@ -1880,10 +1880,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="40">
+      <c r="A23" s="33">
         <v>6</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="36" t="s">
         <v>101</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -1894,16 +1894,16 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="44"/>
+      <c r="A24" s="34"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="44"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="9" t="s">
         <v>45</v>
       </c>
@@ -1912,8 +1912,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="44"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="9" t="s">
         <v>46</v>
       </c>
@@ -1922,8 +1922,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
-      <c r="B27" s="45"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="38"/>
       <c r="C27" s="11"/>
       <c r="D27" s="12" t="s">
         <v>49</v>
@@ -1944,13 +1944,13 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="40">
+      <c r="A29" s="33">
         <v>8</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="41" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="10" t="s">
@@ -1958,62 +1958,62 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="34"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="42"/>
       <c r="D32" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="29"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
+      <c r="A34" s="39">
         <v>9</v>
       </c>
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="47" t="s">
+      <c r="D34" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="40">
+      <c r="A36" s="33">
         <v>10</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="36" t="s">
         <v>107</v>
       </c>
       <c r="C36" s="24" t="s">
@@ -2024,14 +2024,14 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="44"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="17"/>
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="44"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="9" t="s">
         <v>33</v>
       </c>
@@ -2040,24 +2040,24 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="44"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="37"/>
       <c r="C39" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D39" s="15"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="42"/>
-      <c r="B40" s="45"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="22"/>
       <c r="D40" s="16"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="30">
+      <c r="A41" s="39">
         <v>11</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B41" s="27" t="s">
         <v>108</v>
       </c>
       <c r="C41" s="6" t="s">
@@ -2068,14 +2068,14 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="35"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="5" t="s">
         <v>33</v>
       </c>
@@ -2084,64 +2084,64 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="29"/>
       <c r="C45" s="13"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="40">
+      <c r="A46" s="33">
         <v>12</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D46" s="27" t="s">
+      <c r="D46" s="41" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="42"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="30">
+      <c r="A48" s="39">
         <v>13</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C48" s="47" t="s">
+      <c r="C48" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="47" t="s">
+      <c r="D48" s="30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="40">
+      <c r="A50" s="33">
         <v>14</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="36" t="s">
         <v>111</v>
       </c>
       <c r="C50" s="24" t="s">
@@ -2152,14 +2152,14 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="41"/>
-      <c r="B51" s="44"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="37"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="41"/>
-      <c r="B52" s="44"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="37"/>
       <c r="C52" s="9" t="s">
         <v>59</v>
       </c>
@@ -2168,132 +2168,132 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
-      <c r="B53" s="44"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="37"/>
       <c r="C53" s="15"/>
       <c r="D53" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
-      <c r="B54" s="44"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="37"/>
       <c r="C54" s="15"/>
       <c r="D54" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="42"/>
-      <c r="B55" s="45"/>
+      <c r="A55" s="35"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="16"/>
       <c r="D55" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="30">
+      <c r="A56" s="39">
         <v>15</v>
       </c>
-      <c r="B56" s="46" t="s">
+      <c r="B56" s="27" t="s">
         <v>112</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="46" t="s">
+      <c r="D56" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="31"/>
-      <c r="B57" s="35"/>
+      <c r="A57" s="44"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D57" s="35"/>
+      <c r="D57" s="28"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
-      <c r="B58" s="35"/>
+      <c r="A58" s="44"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="35"/>
+      <c r="D58" s="28"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="32"/>
-      <c r="B59" s="36"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="36"/>
+      <c r="D59" s="29"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="40">
+      <c r="A60" s="33">
         <v>16</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="36" t="s">
         <v>113</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D60" s="43" t="s">
+      <c r="D60" s="36" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
-      <c r="B61" s="44"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="37"/>
       <c r="C61" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="44"/>
+      <c r="D61" s="37"/>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="42"/>
-      <c r="B62" s="45"/>
+      <c r="A62" s="35"/>
+      <c r="B62" s="38"/>
       <c r="C62" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D62" s="45"/>
+      <c r="D62" s="38"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="30">
+      <c r="A63" s="39">
         <v>17</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="27" t="s">
         <v>114</v>
       </c>
       <c r="C63" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D63" s="46" t="s">
+      <c r="D63" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
-      <c r="B64" s="35"/>
+      <c r="A64" s="44"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D64" s="35"/>
+      <c r="D64" s="28"/>
     </row>
     <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="32"/>
-      <c r="B65" s="36"/>
+      <c r="A65" s="40"/>
+      <c r="B65" s="29"/>
       <c r="C65" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D65" s="36"/>
+      <c r="D65" s="29"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="40">
+      <c r="A66" s="33">
         <v>18</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="36" t="s">
         <v>115</v>
       </c>
       <c r="C66" s="24" t="s">
@@ -2304,8 +2304,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="41"/>
-      <c r="B67" s="44"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="37"/>
       <c r="C67" s="9" t="s">
         <v>33</v>
       </c>
@@ -2314,46 +2314,46 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="41"/>
-      <c r="B68" s="44"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="37"/>
       <c r="C68" s="9" t="s">
         <v>66</v>
       </c>
       <c r="D68" s="15"/>
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="42"/>
-      <c r="B69" s="45"/>
+      <c r="A69" s="35"/>
+      <c r="B69" s="38"/>
       <c r="C69" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D69" s="16"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="30">
+      <c r="A70" s="39">
         <v>19</v>
       </c>
-      <c r="B70" s="46" t="s">
+      <c r="B70" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C70" s="48" t="s">
+      <c r="C70" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D70" s="46" t="s">
+      <c r="D70" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="32"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="48"/>
-      <c r="D71" s="36"/>
+      <c r="A71" s="40"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="45"/>
+      <c r="D71" s="29"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="40">
+      <c r="A72" s="33">
         <v>20</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="36" t="s">
         <v>117</v>
       </c>
       <c r="C72" s="10" t="s">
@@ -2364,16 +2364,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="41"/>
-      <c r="B73" s="44"/>
+      <c r="A73" s="34"/>
+      <c r="B73" s="37"/>
       <c r="C73" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D73" s="10"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="41"/>
-      <c r="B74" s="44"/>
+      <c r="A74" s="34"/>
+      <c r="B74" s="37"/>
       <c r="C74" s="9" t="s">
         <v>69</v>
       </c>
@@ -2382,8 +2382,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="41"/>
-      <c r="B75" s="44"/>
+      <c r="A75" s="34"/>
+      <c r="B75" s="37"/>
       <c r="C75" s="9" t="s">
         <v>70</v>
       </c>
@@ -2392,406 +2392,387 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="42"/>
-      <c r="B76" s="45"/>
+      <c r="A76" s="35"/>
+      <c r="B76" s="38"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="30">
+      <c r="A77" s="39">
         <v>21</v>
       </c>
-      <c r="B77" s="46" t="s">
+      <c r="B77" s="27" t="s">
         <v>118</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D77" s="47" t="s">
+      <c r="D77" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="31"/>
-      <c r="B78" s="35"/>
+      <c r="A78" s="44"/>
+      <c r="B78" s="28"/>
       <c r="C78" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D78" s="38"/>
+      <c r="D78" s="31"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="31"/>
-      <c r="B79" s="35"/>
+      <c r="A79" s="44"/>
+      <c r="B79" s="28"/>
       <c r="C79" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="38"/>
+      <c r="D79" s="31"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="31"/>
-      <c r="B80" s="35"/>
+      <c r="A80" s="44"/>
+      <c r="B80" s="28"/>
       <c r="C80" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D80" s="38"/>
+      <c r="D80" s="31"/>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="32"/>
-      <c r="B81" s="36"/>
+      <c r="A81" s="40"/>
+      <c r="B81" s="29"/>
       <c r="C81" s="7"/>
-      <c r="D81" s="39"/>
+      <c r="D81" s="32"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="40">
+      <c r="A82" s="33">
         <v>22</v>
       </c>
-      <c r="B82" s="43" t="s">
+      <c r="B82" s="36" t="s">
         <v>119</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D82" s="43" t="s">
+      <c r="D82" s="36" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="41"/>
-      <c r="B83" s="44"/>
+      <c r="A83" s="34"/>
+      <c r="B83" s="37"/>
       <c r="C83" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D83" s="44"/>
+      <c r="D83" s="37"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="41"/>
-      <c r="B84" s="44"/>
+      <c r="A84" s="34"/>
+      <c r="B84" s="37"/>
       <c r="C84" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D84" s="44"/>
+      <c r="D84" s="37"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="41"/>
-      <c r="B85" s="44"/>
+      <c r="A85" s="34"/>
+      <c r="B85" s="37"/>
       <c r="C85" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D85" s="44"/>
+      <c r="D85" s="37"/>
     </row>
     <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="42"/>
-      <c r="B86" s="45"/>
+      <c r="A86" s="35"/>
+      <c r="B86" s="38"/>
       <c r="C86" s="11"/>
-      <c r="D86" s="45"/>
+      <c r="D86" s="38"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="30">
+      <c r="A87" s="39">
         <v>23</v>
       </c>
-      <c r="B87" s="46" t="s">
+      <c r="B87" s="27" t="s">
         <v>120</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D87" s="46" t="s">
+      <c r="D87" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="31"/>
-      <c r="B88" s="35"/>
+      <c r="A88" s="44"/>
+      <c r="B88" s="28"/>
       <c r="C88" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D88" s="35"/>
+      <c r="D88" s="28"/>
     </row>
     <row r="89" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="32"/>
-      <c r="B89" s="36"/>
+      <c r="A89" s="40"/>
+      <c r="B89" s="29"/>
       <c r="C89" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D89" s="36"/>
+      <c r="D89" s="29"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="40">
+      <c r="A90" s="33">
         <v>24</v>
       </c>
-      <c r="B90" s="43" t="s">
+      <c r="B90" s="36" t="s">
         <v>121</v>
       </c>
       <c r="C90" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D90" s="43" t="s">
+      <c r="D90" s="36" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="41"/>
-      <c r="B91" s="44"/>
+      <c r="A91" s="34"/>
+      <c r="B91" s="37"/>
       <c r="C91" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D91" s="44"/>
+      <c r="D91" s="37"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="41"/>
-      <c r="B92" s="44"/>
+      <c r="A92" s="34"/>
+      <c r="B92" s="37"/>
       <c r="C92" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D92" s="44"/>
+      <c r="D92" s="37"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="41"/>
-      <c r="B93" s="44"/>
+      <c r="A93" s="34"/>
+      <c r="B93" s="37"/>
       <c r="C93" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D93" s="44"/>
+      <c r="D93" s="37"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="41"/>
-      <c r="B94" s="44"/>
+      <c r="A94" s="34"/>
+      <c r="B94" s="37"/>
       <c r="C94" s="9"/>
-      <c r="D94" s="44"/>
+      <c r="D94" s="37"/>
     </row>
     <row r="95" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="42"/>
-      <c r="B95" s="45"/>
+      <c r="A95" s="35"/>
+      <c r="B95" s="38"/>
       <c r="C95" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D95" s="45"/>
+      <c r="D95" s="38"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="30">
+      <c r="A96" s="39">
         <v>25</v>
       </c>
-      <c r="B96" s="46" t="s">
+      <c r="B96" s="27" t="s">
         <v>123</v>
       </c>
       <c r="C96" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D96" s="46" t="s">
+      <c r="D96" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="31"/>
-      <c r="B97" s="35"/>
+      <c r="A97" s="44"/>
+      <c r="B97" s="28"/>
       <c r="C97" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D97" s="35"/>
+      <c r="D97" s="28"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="31"/>
-      <c r="B98" s="35"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="28"/>
       <c r="C98" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D98" s="35"/>
+      <c r="D98" s="28"/>
     </row>
     <row r="99" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="32"/>
-      <c r="B99" s="36"/>
+      <c r="A99" s="40"/>
+      <c r="B99" s="29"/>
       <c r="C99" s="7"/>
-      <c r="D99" s="36"/>
+      <c r="D99" s="29"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="40">
+      <c r="A100" s="33">
         <v>26</v>
       </c>
-      <c r="B100" s="43" t="s">
+      <c r="B100" s="36" t="s">
         <v>124</v>
       </c>
       <c r="C100" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D100" s="43" t="s">
+      <c r="D100" s="36" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="41"/>
-      <c r="B101" s="44"/>
+      <c r="A101" s="34"/>
+      <c r="B101" s="37"/>
       <c r="C101" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D101" s="44"/>
+      <c r="D101" s="37"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="41"/>
-      <c r="B102" s="44"/>
+      <c r="A102" s="34"/>
+      <c r="B102" s="37"/>
       <c r="C102" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D102" s="44"/>
+      <c r="D102" s="37"/>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="42"/>
-      <c r="B103" s="45"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="38"/>
       <c r="C103" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D103" s="45"/>
+      <c r="D103" s="38"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="30">
+      <c r="A104" s="39">
         <v>27</v>
       </c>
-      <c r="B104" s="46" t="s">
+      <c r="B104" s="27" t="s">
         <v>125</v>
       </c>
       <c r="C104" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D104" s="46" t="s">
+      <c r="D104" s="27" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="31"/>
-      <c r="B105" s="35"/>
+      <c r="A105" s="44"/>
+      <c r="B105" s="28"/>
       <c r="C105" s="5"/>
-      <c r="D105" s="35"/>
+      <c r="D105" s="28"/>
     </row>
     <row r="106" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="32"/>
-      <c r="B106" s="36"/>
+      <c r="A106" s="40"/>
+      <c r="B106" s="29"/>
       <c r="C106" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D106" s="36"/>
+      <c r="D106" s="29"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="40">
+      <c r="A107" s="33">
         <v>28</v>
       </c>
-      <c r="B107" s="43" t="s">
+      <c r="B107" s="36" t="s">
         <v>126</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D107" s="43" t="s">
+      <c r="D107" s="36" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="41"/>
-      <c r="B108" s="44"/>
+      <c r="A108" s="34"/>
+      <c r="B108" s="37"/>
       <c r="C108" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D108" s="44"/>
+      <c r="D108" s="37"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="41"/>
-      <c r="B109" s="44"/>
+      <c r="A109" s="34"/>
+      <c r="B109" s="37"/>
       <c r="C109" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D109" s="44"/>
+      <c r="D109" s="37"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="41"/>
-      <c r="B110" s="44"/>
+      <c r="A110" s="34"/>
+      <c r="B110" s="37"/>
       <c r="C110" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D110" s="44"/>
+      <c r="D110" s="37"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="41"/>
-      <c r="B111" s="44"/>
+      <c r="A111" s="34"/>
+      <c r="B111" s="37"/>
       <c r="C111" s="9"/>
-      <c r="D111" s="44"/>
+      <c r="D111" s="37"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="41"/>
-      <c r="B112" s="44"/>
+      <c r="A112" s="34"/>
+      <c r="B112" s="37"/>
       <c r="C112" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D112" s="44"/>
+      <c r="D112" s="37"/>
     </row>
     <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="41"/>
-      <c r="B113" s="44"/>
+      <c r="A113" s="34"/>
+      <c r="B113" s="37"/>
       <c r="C113" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D113" s="44"/>
+      <c r="D113" s="37"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="41"/>
-      <c r="B114" s="44"/>
+      <c r="A114" s="34"/>
+      <c r="B114" s="37"/>
       <c r="C114" s="9"/>
-      <c r="D114" s="44"/>
+      <c r="D114" s="37"/>
     </row>
     <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="41"/>
-      <c r="B115" s="44"/>
+      <c r="A115" s="34"/>
+      <c r="B115" s="37"/>
       <c r="C115" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D115" s="44"/>
+      <c r="D115" s="37"/>
     </row>
     <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="42"/>
-      <c r="B116" s="45"/>
+      <c r="A116" s="35"/>
+      <c r="B116" s="38"/>
       <c r="C116" s="11"/>
-      <c r="D116" s="45"/>
+      <c r="D116" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="B104:B106"/>
-    <mergeCell ref="D104:D106"/>
-    <mergeCell ref="A107:A116"/>
-    <mergeCell ref="B107:B116"/>
-    <mergeCell ref="D107:D116"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="D87:D89"/>
-    <mergeCell ref="A90:A95"/>
-    <mergeCell ref="B90:B95"/>
-    <mergeCell ref="D90:D95"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="A50:A55"/>
-    <mergeCell ref="B50:B55"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="B41:B45"/>
     <mergeCell ref="A100:A103"/>
     <mergeCell ref="B100:B103"/>
     <mergeCell ref="D100:D103"/>
@@ -2808,29 +2789,48 @@
     <mergeCell ref="A77:A81"/>
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="B70:B71"/>
+    <mergeCell ref="A87:A89"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="B60:B62"/>
     <mergeCell ref="A60:A62"/>
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="B56:B59"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A50:A55"/>
+    <mergeCell ref="B50:B55"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="D104:D106"/>
+    <mergeCell ref="A107:A116"/>
+    <mergeCell ref="B107:B116"/>
+    <mergeCell ref="D107:D116"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="D87:D89"/>
+    <mergeCell ref="A90:A95"/>
+    <mergeCell ref="B90:B95"/>
+    <mergeCell ref="D90:D95"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="D82:D86"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C115" r:id="rId1" xr:uid="{A92E8291-9674-4699-8238-CD54BFA6A5A0}"/>

</xml_diff>